<commit_message>
text and uart test
add uart and text test
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="91">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -201,6 +201,93 @@
   </si>
   <si>
     <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%s&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;s&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-F,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-F,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z,o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART INIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0xFE</t>
   </si>
 </sst>
 </file>
@@ -1437,9 +1524,15 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
       <c r="I4"/>
       <c r="K4" s="5" t="s">
         <v>17</v>
@@ -1470,9 +1563,15 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>90</v>
+      </c>
       <c r="I5"/>
       <c r="K5" s="8" t="s">
         <v>1</v>
@@ -1501,9 +1600,15 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
       <c r="I6"/>
       <c r="K6" s="8" t="s">
         <v>2</v>
@@ -1677,7 +1782,7 @@
         <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -1717,10 +1822,74 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:10"/>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
-    <row r="10" spans="2:10"/>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="13" spans="2:10"/>
     <row r="14" spans="2:10"/>
     <row r="15" spans="2:10"/>

</xml_diff>